<commit_message>
Adding light support in circuitand default page, adding Excel file to help creating the setup file
</commit_message>
<xml_diff>
--- a/Docs/Creating setup file.xlsx
+++ b/Docs/Creating setup file.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17204"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laurelle\OneDrive\Raspberry PI\LegoTrain\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\LegoTrainDrive\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="102">
   <si>
     <t>Nombre de signaux</t>
   </si>
@@ -260,6 +260,72 @@
   </si>
   <si>
     <t>Key234</t>
+  </si>
+  <si>
+    <t>Signal 1</t>
+  </si>
+  <si>
+    <t>Signal 2</t>
+  </si>
+  <si>
+    <t>milieu</t>
+  </si>
+  <si>
+    <t>Signal 3</t>
+  </si>
+  <si>
+    <t>haut</t>
+  </si>
+  <si>
+    <t>Signal 4</t>
+  </si>
+  <si>
+    <t>bas</t>
+  </si>
+  <si>
+    <t>Signal 5</t>
+  </si>
+  <si>
+    <t>par ici</t>
+  </si>
+  <si>
+    <t>Signal 6</t>
+  </si>
+  <si>
+    <t>par la</t>
+  </si>
+  <si>
+    <t>Signal 7</t>
+  </si>
+  <si>
+    <t>par la bas</t>
+  </si>
+  <si>
+    <t>Signal 8</t>
+  </si>
+  <si>
+    <t>tut en haut</t>
+  </si>
+  <si>
+    <t>Signal</t>
+  </si>
+  <si>
+    <t>Total Signal</t>
+  </si>
+  <si>
+    <t>Number of Signals</t>
+  </si>
+  <si>
+    <t>Number of switchs</t>
+  </si>
+  <si>
+    <t>Number of trains</t>
+  </si>
+  <si>
+    <t>Security key</t>
+  </si>
+  <si>
+    <t>cote gauche</t>
   </si>
 </sst>
 </file>
@@ -665,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +749,7 @@
       </c>
       <c r="B1" s="2" t="str">
         <f>Variables!B21</f>
-        <v>?nsi=6&amp;nai=8&amp;ntr=8&amp;tc1=1&amp;tr1=0&amp;tn1=Marchandise rouge&amp;tv1=5&amp;tc2=1&amp;tr2=1&amp;tn2=Passager rouge&amp;tv2=5&amp;tc3=2&amp;tr3=0&amp;tn3=Marchandise jaune 1&amp;tv3=5&amp;tc4=2&amp;tr4=1&amp;tn4=Marchandise jaune 2&amp;tv4=5&amp;tc5=3&amp;tr5=0&amp;tn5=TGV&amp;tv5=5&amp;tc6=3&amp;tr6=1&amp;tn6=Lumieres TGV&amp;tv6=5&amp;tc7=4&amp;tr7=0&amp;tn7=Herald&amp;tv7=5&amp;tc8=4&amp;tr8=1&amp;tn8=Maersk&amp;tv8=4&amp;ain1=Butte verte&amp;pl1=220&amp;pt1=600&amp;ain2=Grue&amp;pl2=140&amp;pt2=30&amp;ain3=Arbre&amp;pl3=297&amp;pt3=497&amp;ain4=Hobbit&amp;pl4=300&amp;pt4=180&amp;ain5=Depot&amp;pl5=150&amp;pt5=180&amp;ain6=Hobbit&amp;pl6=651&amp;pt6=48&amp;ain7=Police&amp;pl7=137&amp;pt7=497&amp;ain8=Chateau&amp;pl8=566&amp;pt8=556&amp;smi=540&amp;sma=2470&amp;ami=0&amp;ama=180&amp;sa=203&amp;sec=Key234&amp;dbg=0</v>
+        <v>?nsi=8&amp;nai=8&amp;ntr=8&amp;tc1=1&amp;tr1=0&amp;tn1=Marchandise rouge&amp;tv1=5&amp;tc2=1&amp;tr2=1&amp;tn2=Passager rouge&amp;tv2=5&amp;tc3=2&amp;tr3=0&amp;tn3=Marchandise jaune 1&amp;tv3=5&amp;tc4=2&amp;tr4=1&amp;tn4=Marchandise jaune 2&amp;tv4=5&amp;tc5=3&amp;tr5=0&amp;tn5=TGV&amp;tv5=5&amp;tc6=3&amp;tr6=1&amp;tn6=Lumieres TGV&amp;tv6=5&amp;tc7=4&amp;tr7=0&amp;tn7=Herald&amp;tv7=5&amp;tc8=4&amp;tr8=1&amp;tn8=Maersk&amp;tv8=4&amp;ain1=Butte verte&amp;pl1=220&amp;pt1=600&amp;ain2=Grue&amp;pl2=140&amp;pt2=30&amp;ain3=Arbre&amp;pl3=297&amp;pt3=497&amp;ain4=Hobbit&amp;pl4=300&amp;pt4=180&amp;ain5=Depot&amp;pl5=150&amp;pt5=180&amp;ain6=Hobbit&amp;pl6=651&amp;pt6=48&amp;ain7=Police&amp;pl7=137&amp;pt7=497&amp;ain8=Chateau&amp;pl8=566&amp;pt8=556&amp;smi=800&amp;sma=2190&amp;ami=0&amp;ama=180&amp;sa=203&amp;tr1=cote gauche&amp;spl1=200&amp;spt1=550&amp;tr2=milieu&amp;spl2=120&amp;spt2=10&amp;tr3=haut&amp;spl3=279&amp;spt3=523&amp;tr4=bas&amp;spl4=250&amp;spt4=160&amp;tr5=par ici&amp;spl5=130&amp;spt5=160&amp;tr6=par la&amp;spl6=33&amp;spt6=645&amp;tr7=par la bas&amp;spl7=127&amp;spt7=457&amp;tr8=tut en haut&amp;spl8=536&amp;spt8=546&amp;sec=Key234&amp;dbg=0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -702,15 +768,15 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="B5" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="B6" s="1">
         <v>8</v>
@@ -718,7 +784,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="B7" s="1">
         <v>8</v>
@@ -726,7 +792,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>79</v>
@@ -1009,51 +1075,175 @@
         <v>566</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B30" s="1">
-        <v>0</v>
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="5">
+        <v>200</v>
+      </c>
+      <c r="D30" s="5">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="5">
+        <v>120</v>
+      </c>
+      <c r="D31" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="5">
+        <v>279</v>
+      </c>
+      <c r="D32" s="5">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="5">
+        <v>250</v>
+      </c>
+      <c r="D33" s="5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" s="5">
+        <v>130</v>
+      </c>
+      <c r="D34" s="5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="5">
+        <v>33</v>
+      </c>
+      <c r="D35" s="5">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="5">
+        <v>127</v>
+      </c>
+      <c r="D36" s="5">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="5">
+        <v>536</v>
+      </c>
+      <c r="D37" s="5">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B32" s="1">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="B41" s="1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B33" s="1">
-        <v>2470</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="B42" s="1">
+        <v>2190</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B43" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B44" s="1">
         <v>180</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B45" s="1">
         <v>203</v>
       </c>
     </row>
@@ -1095,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C44"/>
+  <dimension ref="A2:C54"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,8 +1434,8 @@
         <v>28</v>
       </c>
       <c r="B21" t="str">
-        <f>B22&amp;B32&amp;B42&amp;B44&amp;Variables!B12&amp;"="&amp;Paramétrage!B8&amp;"&amp;"&amp;B13&amp;"="&amp;Paramétrage!B30</f>
-        <v>?nsi=6&amp;nai=8&amp;ntr=8&amp;tc1=1&amp;tr1=0&amp;tn1=Marchandise rouge&amp;tv1=5&amp;tc2=1&amp;tr2=1&amp;tn2=Passager rouge&amp;tv2=5&amp;tc3=2&amp;tr3=0&amp;tn3=Marchandise jaune 1&amp;tv3=5&amp;tc4=2&amp;tr4=1&amp;tn4=Marchandise jaune 2&amp;tv4=5&amp;tc5=3&amp;tr5=0&amp;tn5=TGV&amp;tv5=5&amp;tc6=3&amp;tr6=1&amp;tn6=Lumieres TGV&amp;tv6=5&amp;tc7=4&amp;tr7=0&amp;tn7=Herald&amp;tv7=5&amp;tc8=4&amp;tr8=1&amp;tn8=Maersk&amp;tv8=4&amp;ain1=Butte verte&amp;pl1=220&amp;pt1=600&amp;ain2=Grue&amp;pl2=140&amp;pt2=30&amp;ain3=Arbre&amp;pl3=297&amp;pt3=497&amp;ain4=Hobbit&amp;pl4=300&amp;pt4=180&amp;ain5=Depot&amp;pl5=150&amp;pt5=180&amp;ain6=Hobbit&amp;pl6=651&amp;pt6=48&amp;ain7=Police&amp;pl7=137&amp;pt7=497&amp;ain8=Chateau&amp;pl8=566&amp;pt8=556&amp;smi=540&amp;sma=2470&amp;ami=0&amp;ama=180&amp;sa=203&amp;sec=Key234&amp;dbg=0</v>
+        <f>B22&amp;B32&amp;B42&amp;B44&amp;B54&amp;Variables!B12&amp;"="&amp;Paramétrage!B8&amp;"&amp;"&amp;B13&amp;"="&amp;Paramétrage!B39</f>
+        <v>?nsi=8&amp;nai=8&amp;ntr=8&amp;tc1=1&amp;tr1=0&amp;tn1=Marchandise rouge&amp;tv1=5&amp;tc2=1&amp;tr2=1&amp;tn2=Passager rouge&amp;tv2=5&amp;tc3=2&amp;tr3=0&amp;tn3=Marchandise jaune 1&amp;tv3=5&amp;tc4=2&amp;tr4=1&amp;tn4=Marchandise jaune 2&amp;tv4=5&amp;tc5=3&amp;tr5=0&amp;tn5=TGV&amp;tv5=5&amp;tc6=3&amp;tr6=1&amp;tn6=Lumieres TGV&amp;tv6=5&amp;tc7=4&amp;tr7=0&amp;tn7=Herald&amp;tv7=5&amp;tc8=4&amp;tr8=1&amp;tn8=Maersk&amp;tv8=4&amp;ain1=Butte verte&amp;pl1=220&amp;pt1=600&amp;ain2=Grue&amp;pl2=140&amp;pt2=30&amp;ain3=Arbre&amp;pl3=297&amp;pt3=497&amp;ain4=Hobbit&amp;pl4=300&amp;pt4=180&amp;ain5=Depot&amp;pl5=150&amp;pt5=180&amp;ain6=Hobbit&amp;pl6=651&amp;pt6=48&amp;ain7=Police&amp;pl7=137&amp;pt7=497&amp;ain8=Chateau&amp;pl8=566&amp;pt8=556&amp;smi=800&amp;sma=2190&amp;ami=0&amp;ama=180&amp;sa=203&amp;tr1=cote gauche&amp;spl1=200&amp;spt1=550&amp;tr2=milieu&amp;spl2=120&amp;spt2=10&amp;tr3=haut&amp;spl3=279&amp;spt3=523&amp;tr4=bas&amp;spl4=250&amp;spt4=160&amp;tr5=par ici&amp;spl5=130&amp;spt5=160&amp;tr6=par la&amp;spl6=33&amp;spt6=645&amp;tr7=par la bas&amp;spl7=127&amp;spt7=457&amp;tr8=tut en haut&amp;spl8=536&amp;spt8=546&amp;sec=Key234&amp;dbg=0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1254,7 +1444,7 @@
       </c>
       <c r="B22" s="2" t="str">
         <f>"?"&amp;Variables!B5&amp;"="&amp;Paramétrage!B5&amp;"&amp;"&amp;Variables!B6&amp;"="&amp;Paramétrage!B6&amp;"&amp;"&amp;Variables!B7&amp;"="&amp;Paramétrage!B7</f>
-        <v>?nsi=6&amp;nai=8&amp;ntr=8</v>
+        <v>?nsi=8&amp;nai=8&amp;ntr=8</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1467,8 +1657,94 @@
         <v>71</v>
       </c>
       <c r="B44" t="str">
-        <f>B15&amp;"="&amp;Paramétrage!B32&amp;"&amp;"&amp;Variables!B16&amp;"="&amp;Paramétrage!B33&amp;"&amp;"&amp;Variables!B17&amp;"="&amp;Paramétrage!B34&amp;"&amp;"&amp;Variables!B18&amp;"="&amp;Paramétrage!B35&amp;"&amp;"&amp;B19&amp;"="&amp;Paramétrage!B36&amp;"&amp;"</f>
-        <v>smi=540&amp;sma=2470&amp;ami=0&amp;ama=180&amp;sa=203&amp;</v>
+        <f>B15&amp;"="&amp;Paramétrage!B41&amp;"&amp;"&amp;Variables!B16&amp;"="&amp;Paramétrage!B42&amp;"&amp;"&amp;Variables!B17&amp;"="&amp;Paramétrage!B43&amp;"&amp;"&amp;Variables!B18&amp;"="&amp;Paramétrage!B44&amp;"&amp;"&amp;B19&amp;"="&amp;Paramétrage!B45&amp;"&amp;"</f>
+        <v>smi=800&amp;sma=2190&amp;ami=0&amp;ama=180&amp;sa=203&amp;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="str">
+        <f>$B$11&amp;Variables!A46&amp;"="&amp;Paramétrage!B30&amp;"&amp;"&amp;"spl"&amp;A46&amp;"="&amp;Paramétrage!C30&amp;"&amp;spt"&amp;A46&amp;"="&amp;Paramétrage!D30&amp;"&amp;"</f>
+        <v>tr1=cote gauche&amp;spl1=200&amp;spt1=550&amp;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47" t="str">
+        <f>$B$11&amp;Variables!A47&amp;"="&amp;Paramétrage!B31&amp;"&amp;"&amp;"spl"&amp;A47&amp;"="&amp;Paramétrage!C31&amp;"&amp;spt"&amp;A47&amp;"="&amp;Paramétrage!D31&amp;"&amp;"</f>
+        <v>tr2=milieu&amp;spl2=120&amp;spt2=10&amp;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48" t="str">
+        <f>$B$11&amp;Variables!A48&amp;"="&amp;Paramétrage!B32&amp;"&amp;"&amp;"spl"&amp;A48&amp;"="&amp;Paramétrage!C32&amp;"&amp;spt"&amp;A48&amp;"="&amp;Paramétrage!D32&amp;"&amp;"</f>
+        <v>tr3=haut&amp;spl3=279&amp;spt3=523&amp;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>4</v>
+      </c>
+      <c r="B49" t="str">
+        <f>$B$11&amp;Variables!A49&amp;"="&amp;Paramétrage!B33&amp;"&amp;"&amp;"spl"&amp;A49&amp;"="&amp;Paramétrage!C33&amp;"&amp;spt"&amp;A49&amp;"="&amp;Paramétrage!D33&amp;"&amp;"</f>
+        <v>tr4=bas&amp;spl4=250&amp;spt4=160&amp;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>5</v>
+      </c>
+      <c r="B50" t="str">
+        <f>$B$11&amp;Variables!A50&amp;"="&amp;Paramétrage!B34&amp;"&amp;"&amp;"spl"&amp;A50&amp;"="&amp;Paramétrage!C34&amp;"&amp;spt"&amp;A50&amp;"="&amp;Paramétrage!D34&amp;"&amp;"</f>
+        <v>tr5=par ici&amp;spl5=130&amp;spt5=160&amp;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>6</v>
+      </c>
+      <c r="B51" t="str">
+        <f>$B$11&amp;Variables!A51&amp;"="&amp;Paramétrage!B35&amp;"&amp;"&amp;"spl"&amp;A51&amp;"="&amp;Paramétrage!C35&amp;"&amp;spt"&amp;A51&amp;"="&amp;Paramétrage!D35&amp;"&amp;"</f>
+        <v>tr6=par la&amp;spl6=33&amp;spt6=645&amp;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>7</v>
+      </c>
+      <c r="B52" t="str">
+        <f>$B$11&amp;Variables!A52&amp;"="&amp;Paramétrage!B36&amp;"&amp;"&amp;"spl"&amp;A52&amp;"="&amp;Paramétrage!C36&amp;"&amp;spt"&amp;A52&amp;"="&amp;Paramétrage!D36&amp;"&amp;"</f>
+        <v>tr7=par la bas&amp;spl7=127&amp;spt7=457&amp;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>8</v>
+      </c>
+      <c r="B53" t="str">
+        <f>$B$11&amp;Variables!A53&amp;"="&amp;Paramétrage!B37&amp;"&amp;"&amp;"spl"&amp;A53&amp;"="&amp;Paramétrage!C37&amp;"&amp;spt"&amp;A53&amp;"="&amp;Paramétrage!D37&amp;"&amp;"</f>
+        <v>tr8=tut en haut&amp;spl8=536&amp;spt8=546&amp;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" t="str">
+        <f>B46&amp;B47&amp;B48&amp;B49&amp;B50&amp;B51&amp;B52&amp;B53</f>
+        <v>tr1=cote gauche&amp;spl1=200&amp;spt1=550&amp;tr2=milieu&amp;spl2=120&amp;spt2=10&amp;tr3=haut&amp;spl3=279&amp;spt3=523&amp;tr4=bas&amp;spl4=250&amp;spt4=160&amp;tr5=par ici&amp;spl5=130&amp;spt5=160&amp;tr6=par la&amp;spl6=33&amp;spt6=645&amp;tr7=par la bas&amp;spl7=127&amp;spt7=457&amp;tr8=tut en haut&amp;spl8=536&amp;spt8=546&amp;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>